<commit_message>
login, reports, delete then submit
</commit_message>
<xml_diff>
--- a/friendOdds.xlsx
+++ b/friendOdds.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamcowart/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamcowart/Documents/friendOdds/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" tabRatio="500"/>
+    <workbookView xWindow="4800" yWindow="460" windowWidth="28800" windowHeight="16620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="158">
   <si>
     <t>sport</t>
   </si>
@@ -160,13 +160,352 @@
   </si>
   <si>
     <t>MUN/SEV</t>
+  </si>
+  <si>
+    <t>EPL</t>
+  </si>
+  <si>
+    <t>Southampton</t>
+  </si>
+  <si>
+    <t>Chelsea</t>
+  </si>
+  <si>
+    <t>CHELSEA</t>
+  </si>
+  <si>
+    <t>-½ (-115)</t>
+  </si>
+  <si>
+    <t>200082</t>
+  </si>
+  <si>
+    <t>SOUTHAMPTON</t>
+  </si>
+  <si>
+    <t>+½ (-115)</t>
+  </si>
+  <si>
+    <t>200083</t>
+  </si>
+  <si>
+    <t>DRAW</t>
+  </si>
+  <si>
+    <t>EVERTON</t>
+  </si>
+  <si>
+    <t>o2½ (+135)</t>
+  </si>
+  <si>
+    <t>PK (EVEN)</t>
+  </si>
+  <si>
+    <t>SWANSEA CITY</t>
+  </si>
+  <si>
+    <t>u2½ (-165)</t>
+  </si>
+  <si>
+    <t>PK (-130)</t>
+  </si>
+  <si>
+    <t>WATFORD</t>
+  </si>
+  <si>
+    <t>o2½ (+120)</t>
+  </si>
+  <si>
+    <t>PK (-115)</t>
+  </si>
+  <si>
+    <t>HUDDERSFIELD TOWN</t>
+  </si>
+  <si>
+    <t>u2½ (-150)</t>
+  </si>
+  <si>
+    <t>BRIGHTON &amp; HOVE ALBION</t>
+  </si>
+  <si>
+    <t>200094</t>
+  </si>
+  <si>
+    <t>CRYSTAL PALACE</t>
+  </si>
+  <si>
+    <t>200095</t>
+  </si>
+  <si>
+    <t>LEICESTER CITY</t>
+  </si>
+  <si>
+    <t>o2 (-130)</t>
+  </si>
+  <si>
+    <t>BURNLEY FC</t>
+  </si>
+  <si>
+    <t>u2 (EVEN)</t>
+  </si>
+  <si>
+    <t>BOURNEMOUTH</t>
+  </si>
+  <si>
+    <t>o3½ (-105)</t>
+  </si>
+  <si>
+    <t>+2 (-140)</t>
+  </si>
+  <si>
+    <t>LIVERPOOL</t>
+  </si>
+  <si>
+    <t>u3½ (-125)</t>
+  </si>
+  <si>
+    <t>-2 (+110)</t>
+  </si>
+  <si>
+    <t>MANCHESTER CITY</t>
+  </si>
+  <si>
+    <t>o3 (-110)</t>
+  </si>
+  <si>
+    <t>TOTTENHAM</t>
+  </si>
+  <si>
+    <t>u3 (-120)</t>
+  </si>
+  <si>
+    <t>+.5</t>
+  </si>
+  <si>
+    <t>-.5</t>
+  </si>
+  <si>
+    <t>-115</t>
+  </si>
+  <si>
+    <t>+260</t>
+  </si>
+  <si>
+    <t>SOT/CHE</t>
+  </si>
+  <si>
+    <t>2018-04-18</t>
+  </si>
+  <si>
+    <t>Swansea City</t>
+  </si>
+  <si>
+    <t>Everton</t>
+  </si>
+  <si>
+    <t>+150</t>
+  </si>
+  <si>
+    <t>+205</t>
+  </si>
+  <si>
+    <t>PK</t>
+  </si>
+  <si>
+    <t>-130</t>
+  </si>
+  <si>
+    <t>EVEN</t>
+  </si>
+  <si>
+    <t>u2.5</t>
+  </si>
+  <si>
+    <t>o2.5</t>
+  </si>
+  <si>
+    <t>+135</t>
+  </si>
+  <si>
+    <t>-165</t>
+  </si>
+  <si>
+    <t>+220</t>
+  </si>
+  <si>
+    <t>SWA/EVE</t>
+  </si>
+  <si>
+    <t>Huddersfield Town</t>
+  </si>
+  <si>
+    <t>Watford</t>
+  </si>
+  <si>
+    <t>+165</t>
+  </si>
+  <si>
+    <t>+185</t>
+  </si>
+  <si>
+    <t>-150</t>
+  </si>
+  <si>
+    <t>+215</t>
+  </si>
+  <si>
+    <t>HUD/WAT</t>
+  </si>
+  <si>
+    <t>Crystal Palace</t>
+  </si>
+  <si>
+    <t>Brightone &amp; Hove Albion</t>
+  </si>
+  <si>
+    <t>+235</t>
+  </si>
+  <si>
+    <t>CRY/BHA</t>
+  </si>
+  <si>
+    <t>Burnley</t>
+  </si>
+  <si>
+    <t>Leicester City</t>
+  </si>
+  <si>
+    <t>o2</t>
+  </si>
+  <si>
+    <t>u2</t>
+  </si>
+  <si>
+    <t>+210</t>
+  </si>
+  <si>
+    <t>BUR/LEI</t>
+  </si>
+  <si>
+    <t>Bournemouth</t>
+  </si>
+  <si>
+    <t>-405</t>
+  </si>
+  <si>
+    <t>+1100</t>
+  </si>
+  <si>
+    <t>-2</t>
+  </si>
+  <si>
+    <t>-125</t>
+  </si>
+  <si>
+    <t>+530</t>
+  </si>
+  <si>
+    <t>LIV/BOU</t>
+  </si>
+  <si>
+    <t>Tottenham</t>
+  </si>
+  <si>
+    <t>+160</t>
+  </si>
+  <si>
+    <t>-110</t>
+  </si>
+  <si>
+    <t>-120</t>
+  </si>
+  <si>
+    <t>+255</t>
+  </si>
+  <si>
+    <t>TOT/MCI</t>
+  </si>
+  <si>
+    <t>2018-04-14</t>
+  </si>
+  <si>
+    <t>2018-04-15</t>
+  </si>
+  <si>
+    <t>Newcastle United</t>
+  </si>
+  <si>
+    <t>Arsenal</t>
+  </si>
+  <si>
+    <t>+110</t>
+  </si>
+  <si>
+    <t>NEW/ARS</t>
+  </si>
+  <si>
+    <t>Manchested United</t>
+  </si>
+  <si>
+    <t>West Brom</t>
+  </si>
+  <si>
+    <t>-590</t>
+  </si>
+  <si>
+    <t>+1680</t>
+  </si>
+  <si>
+    <t>-145</t>
+  </si>
+  <si>
+    <t>+115</t>
+  </si>
+  <si>
+    <t>+635</t>
+  </si>
+  <si>
+    <t>MUN/WBA</t>
+  </si>
+  <si>
+    <t>2018-04-16</t>
+  </si>
+  <si>
+    <t>West Ham</t>
+  </si>
+  <si>
+    <t>Stoke City</t>
+  </si>
+  <si>
+    <t>+295</t>
+  </si>
+  <si>
+    <t>+240</t>
+  </si>
+  <si>
+    <t>WHA/STO</t>
+  </si>
+  <si>
+    <t>2018-04-17</t>
+  </si>
+  <si>
+    <t>Brighton &amp; Hove Albion</t>
+  </si>
+  <si>
+    <t>Manchester United</t>
+  </si>
+  <si>
+    <t>2018-04-19</t>
+  </si>
+  <si>
+    <t>Southamption</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -181,6 +520,25 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -203,11 +561,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,31 +847,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.6640625" customWidth="1"/>
-    <col min="17" max="17" width="198.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="230.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -525,37 +887,37 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
@@ -776,6 +1138,508 @@
       <c r="Q5" t="str">
         <f t="shared" si="0"/>
         <v>insert into games values (id,'Champions League','2018-04-10','Bayern Munich','Sevilla','Bayern Munich -450','Sevilla +1220','Bayern Munich -2','-115','Sevilla +2','-115','MUN/SEV o3.5','-115','MUN/SEV u3.5','-115','Draw MUN/SEV +550',NULL,NULL,NULL,NULL,NULL,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="3">
+        <v>-115</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" t="s">
+        <v>104</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" t="s">
+        <v>111</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>120</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C13" t="s">
+        <v>127</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D14" t="s">
+        <v>136</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15" t="s">
+        <v>139</v>
+      </c>
+      <c r="D15" t="s">
+        <v>140</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C16" t="s">
+        <v>148</v>
+      </c>
+      <c r="D16" t="s">
+        <v>149</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C17" t="s">
+        <v>154</v>
+      </c>
+      <c r="D17" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C19" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C20" t="s">
+        <v>115</v>
+      </c>
+      <c r="D20" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -785,12 +1649,342 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="4">
+        <v>43204.3125</v>
+      </c>
+      <c r="B1">
+        <v>200081</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1">
+        <v>-115</v>
+      </c>
+      <c r="F1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2">
+        <v>335</v>
+      </c>
+      <c r="E2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>43204.416666666664</v>
+      </c>
+      <c r="B4">
+        <v>200085</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4">
+        <v>205</v>
+      </c>
+      <c r="E4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>200086</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5">
+        <v>150</v>
+      </c>
+      <c r="D5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>200087</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>43204.416666666664</v>
+      </c>
+      <c r="B7">
+        <v>200089</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7">
+        <v>185</v>
+      </c>
+      <c r="E7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>200090</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8">
+        <v>165</v>
+      </c>
+      <c r="D8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>200091</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>43204.416666666664</v>
+      </c>
+      <c r="B10">
+        <v>200093</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10">
+        <v>320</v>
+      </c>
+      <c r="F10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11">
+        <v>-105</v>
+      </c>
+      <c r="E11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>43204.416666666664</v>
+      </c>
+      <c r="B13">
+        <v>200097</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13">
+        <v>185</v>
+      </c>
+      <c r="E13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>200098</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14">
+        <v>165</v>
+      </c>
+      <c r="D14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>200099</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
+        <v>43204.520833333336</v>
+      </c>
+      <c r="B16">
+        <v>200101</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16">
+        <v>1100</v>
+      </c>
+      <c r="E16" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>200102</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17">
+        <v>-405</v>
+      </c>
+      <c r="D17" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>200103</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
+        <v>43204.614583333336</v>
+      </c>
+      <c r="B19">
+        <v>200105</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19">
+        <v>160</v>
+      </c>
+      <c r="E19" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>200106</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20">
+        <v>165</v>
+      </c>
+      <c r="D20" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="6">
+        <v>200107</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="6">
+        <v>255</v>
+      </c>
+      <c r="D21" s="6"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>